<commit_message>
Update: Threat Alert Report - 2026-01-11 01:17
</commit_message>
<xml_diff>
--- a/excel_routes/route_AJF_CAI_threats.xlsx
+++ b/excel_routes/route_AJF_CAI_threats.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,7 +528,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>08-JAN-26</t>
+          <t>15-JAN-26</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -542,13 +542,13 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>600</v>
+        <v>421</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>668</v>
+        <v>458</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>-68</v>
+        <v>-37</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>30</v>
@@ -565,51 +565,6 @@
         </is>
       </c>
       <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>SAR</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>05-MAR-26</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>SM-322</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Nile Air NP-120</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>950</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>998</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>-48</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="H3" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="3" t="inlineStr">
-        <is>
-          <t>LOW THREAT</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="inlineStr">
         <is>
           <t>SAR</t>
         </is>

</xml_diff>